<commit_message>
Code couleur et ajout de panda3D dans le comparatif logiciel
</commit_message>
<xml_diff>
--- a/1 - Avant Projet/3 - Études/1 - Comparatif Logiciels.xlsx
+++ b/1 - Avant Projet/3 - Études/1 - Comparatif Logiciels.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillaume\Desktop\MEGAsync\Cours MMI\S2\PTUT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Serious-Game-MMI\1 - Avant Projet\3 - Études\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
     <t>Unity</t>
   </si>
@@ -126,13 +126,28 @@
   </si>
   <si>
     <t>Gratuit (très limité)</t>
+  </si>
+  <si>
+    <t>Panda 3D</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>Win., Mac OS X, Ubuntu, Debian, Fedora</t>
+  </si>
+  <si>
+    <t>1/5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,20 +157,85 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -163,16 +243,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -485,227 +630,309 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="16" t="s">
         <v>33</v>
       </c>
+      <c r="I2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H8" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
+      <c r="I8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changement de quelques notes dans le comparatif logiciel
</commit_message>
<xml_diff>
--- a/1 - Avant Projet/3 - Études/1 - Comparatif Logiciels.xlsx
+++ b/1 - Avant Projet/3 - Études/1 - Comparatif Logiciels.xlsx
@@ -147,7 +147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +211,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -265,21 +272,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -307,10 +302,10 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -633,7 +628,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,29 +644,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J1" s="1"/>
@@ -683,31 +678,31 @@
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="J2" s="1"/>
@@ -719,31 +714,31 @@
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J3" s="1"/>
@@ -755,31 +750,31 @@
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="8" t="s">
         <v>38</v>
       </c>
       <c r="J4" s="1"/>
@@ -791,31 +786,31 @@
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="8" t="s">
         <v>36</v>
       </c>
       <c r="J5" s="1"/>
@@ -827,31 +822,31 @@
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="J6" s="1"/>
@@ -863,31 +858,31 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="7" t="s">
         <v>37</v>
       </c>
       <c r="J7" s="1"/>
@@ -899,31 +894,31 @@
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="7" t="s">
         <v>35</v>
       </c>
       <c r="J8" s="1"/>

</xml_diff>